<commit_message>
fix logger for backend apps
</commit_message>
<xml_diff>
--- a/client/react/benchmarks.xlsx
+++ b/client/react/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Code\hype\BENCHMARKS\client\react\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D78CA6-520F-4ECC-A9D2-BC1421311810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EE7584-F093-413C-BD92-012E35C60853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +573,10 @@
         <f>MIN(C2:G2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2">
+        <f>MAX(C2:G2)</f>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>